<commit_message>
[VSW][APP] Make test case #19
[ISSUE] VSW # 19
[DES] Complete make test case.
</commit_message>
<xml_diff>
--- a/Document/TEST CASE-VietnameseSpecialWebsite...xlsx
+++ b/Document/TEST CASE-VietnameseSpecialWebsite...xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="180" windowWidth="19440" windowHeight="7575" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="19440" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="1" r:id="rId1"/>
@@ -41,14 +41,14 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="hoahtn6052 - Personal View" guid="{FD5FE319-AD9E-494D-BEEE-D43E425D7630}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1360" windowHeight="547" activeSheetId="9"/>
     <customWorkbookView name="anhdt6087 - Personal View" guid="{F1FB9E11-3D79-46CC-BED1-C4F060AFC065}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1366" windowHeight="573" activeSheetId="5" showFormulaBar="0"/>
-    <customWorkbookView name="hoahtn6052 - Personal View" guid="{FD5FE319-AD9E-494D-BEEE-D43E425D7630}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1360" windowHeight="547" activeSheetId="9"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="601">
   <si>
     <t>Reviewer</t>
   </si>
@@ -3249,6 +3249,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Order management</t>
+  </si>
+  <si>
+    <t>HoaDT48</t>
   </si>
 </sst>
 </file>
@@ -6212,6 +6215,36 @@
     <xf numFmtId="164" fontId="34" fillId="37" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="26" fillId="30" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="30" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="30" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="30" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="30" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="30" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="27" borderId="16" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="27" borderId="17" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="28" borderId="18" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="28" borderId="22" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="28" fillId="28" borderId="58" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -6266,12 +6299,6 @@
     <xf numFmtId="164" fontId="28" fillId="28" borderId="15" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="27" borderId="16" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="27" borderId="17" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="28" fillId="28" borderId="18" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -6283,135 +6310,6 @@
     </xf>
     <xf numFmtId="164" fontId="28" fillId="28" borderId="21" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="30" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="30" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="30" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="30" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="30" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="30" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="28" borderId="18" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="28" borderId="22" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="24" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="27" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="27" borderId="11" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="12" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="13" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="14" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="15" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="27" borderId="16" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="27" borderId="17" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="18" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="19" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="20" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="21" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="30" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="30" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="30" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="30" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="30" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="30" borderId="100" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="33" borderId="101" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="33" borderId="102" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="33" borderId="103" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="28" borderId="18" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="28" borderId="22" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="58" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="59" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="28" borderId="60" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="29" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="29" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="29" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="29" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="30" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="30" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="28" borderId="26" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="28" borderId="27" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6466,6 +6364,111 @@
     </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="120" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="30" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="30" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="30" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="30" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="30" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="30" borderId="100" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="33" borderId="101" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="33" borderId="102" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="33" borderId="103" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="27" borderId="16" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="27" borderId="17" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="28" borderId="18" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="28" borderId="22" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="58" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="59" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="60" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="29" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="29" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="29" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="29" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="30" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="30" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="28" borderId="26" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="28" borderId="27" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="24" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="27" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="27" borderId="11" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="12" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="13" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="14" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="15" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="18" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="19" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="20" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="28" borderId="21" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="121" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7126,7 +7129,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -7281,7 +7284,9 @@
       <c r="C11" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="39" t="s">
+        <v>600</v>
+      </c>
       <c r="E11" s="37" t="s">
         <v>1</v>
       </c>
@@ -7600,12 +7605,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F1FB9E11-3D79-46CC-BED1-C4F060AFC065}">
+    <customSheetView guid="{FD5FE319-AD9E-494D-BEEE-D43E425D7630}">
       <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{FD5FE319-AD9E-494D-BEEE-D43E425D7630}">
+    <customSheetView guid="{F1FB9E11-3D79-46CC-BED1-C4F060AFC065}">
       <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7623,7 +7628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -7637,10 +7642,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="321" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="279"/>
+      <c r="B1" s="321"/>
       <c r="C1" s="208"/>
       <c r="D1" s="208"/>
       <c r="E1" s="140"/>
@@ -7650,81 +7655,81 @@
       <c r="I1" s="143"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="280" t="s">
+      <c r="A2" s="322" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="281"/>
+      <c r="B2" s="323"/>
       <c r="C2" s="144"/>
-      <c r="D2" s="282" t="s">
+      <c r="D2" s="324" t="s">
         <v>230</v>
       </c>
-      <c r="E2" s="283"/>
-      <c r="F2" s="283"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="285"/>
+      <c r="E2" s="325"/>
+      <c r="F2" s="325"/>
+      <c r="G2" s="326"/>
+      <c r="H2" s="326"/>
+      <c r="I2" s="327"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="286" t="s">
+      <c r="A3" s="306" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="287"/>
+      <c r="B3" s="307"/>
       <c r="C3" s="145"/>
-      <c r="D3" s="288" t="s">
+      <c r="D3" s="328" t="s">
         <v>530</v>
       </c>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="290"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="291"/>
+      <c r="E3" s="329"/>
+      <c r="F3" s="329"/>
+      <c r="G3" s="330"/>
+      <c r="H3" s="330"/>
+      <c r="I3" s="331"/>
     </row>
     <row r="4" spans="1:9" ht="25.5">
-      <c r="A4" s="286" t="s">
+      <c r="A4" s="306" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="287"/>
+      <c r="B4" s="307"/>
       <c r="C4" s="145"/>
-      <c r="D4" s="301" t="s">
+      <c r="D4" s="308" t="s">
         <v>229</v>
       </c>
-      <c r="E4" s="302"/>
+      <c r="E4" s="309"/>
       <c r="F4" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="303"/>
-      <c r="H4" s="304"/>
-      <c r="I4" s="305"/>
+      <c r="G4" s="310"/>
+      <c r="H4" s="311"/>
+      <c r="I4" s="312"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="306" t="s">
+      <c r="A5" s="313" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="307"/>
-      <c r="C5" s="307"/>
-      <c r="D5" s="307"/>
-      <c r="E5" s="307"/>
-      <c r="F5" s="307"/>
-      <c r="G5" s="308"/>
-      <c r="H5" s="308"/>
-      <c r="I5" s="309"/>
+      <c r="B5" s="314"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="314"/>
+      <c r="E5" s="314"/>
+      <c r="F5" s="314"/>
+      <c r="G5" s="315"/>
+      <c r="H5" s="315"/>
+      <c r="I5" s="316"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="310" t="s">
+      <c r="A6" s="317" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="311"/>
+      <c r="B6" s="318"/>
       <c r="C6" s="147"/>
       <c r="D6" s="148"/>
       <c r="E6" s="149"/>
       <c r="F6" s="149"/>
-      <c r="G6" s="312"/>
-      <c r="H6" s="312"/>
-      <c r="I6" s="313"/>
+      <c r="G6" s="319"/>
+      <c r="H6" s="319"/>
+      <c r="I6" s="320"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="292"/>
-      <c r="B7" s="293"/>
+      <c r="A7" s="297"/>
+      <c r="B7" s="298"/>
       <c r="C7" s="147"/>
       <c r="D7" s="150" t="s">
         <v>7</v>
@@ -7742,10 +7747,10 @@
       <c r="I7" s="142"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="294" t="s">
+      <c r="A8" s="299" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="295"/>
+      <c r="B8" s="300"/>
       <c r="C8" s="154"/>
       <c r="D8" s="148">
         <f>COUNTIF(G12:G14,"Passed")</f>
@@ -7767,10 +7772,10 @@
       <c r="I8" s="142"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="296" t="s">
+      <c r="A9" s="301" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="297"/>
+      <c r="B9" s="302"/>
       <c r="C9" s="155"/>
       <c r="D9" s="156">
         <f xml:space="preserve"> COUNTIF(H12:H14,"Passed")</f>
@@ -7821,17 +7826,17 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="298" t="s">
+      <c r="A11" s="303" t="s">
         <v>531</v>
       </c>
-      <c r="B11" s="299"/>
-      <c r="C11" s="299"/>
-      <c r="D11" s="299"/>
-      <c r="E11" s="299"/>
-      <c r="F11" s="299"/>
-      <c r="G11" s="299"/>
-      <c r="H11" s="299"/>
-      <c r="I11" s="300"/>
+      <c r="B11" s="304"/>
+      <c r="C11" s="304"/>
+      <c r="D11" s="304"/>
+      <c r="E11" s="304"/>
+      <c r="F11" s="304"/>
+      <c r="G11" s="304"/>
+      <c r="H11" s="304"/>
+      <c r="I11" s="305"/>
     </row>
     <row r="12" spans="1:9" ht="63" customHeight="1">
       <c r="A12" s="161">
@@ -7855,23 +7860,23 @@
       <c r="I12" s="162"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="315" t="s">
+      <c r="A13" s="280" t="s">
         <v>333</v>
       </c>
-      <c r="B13" s="316"/>
-      <c r="C13" s="316"/>
-      <c r="D13" s="316"/>
-      <c r="E13" s="316"/>
-      <c r="F13" s="316"/>
-      <c r="G13" s="316"/>
-      <c r="H13" s="316"/>
-      <c r="I13" s="317"/>
+      <c r="B13" s="281"/>
+      <c r="C13" s="281"/>
+      <c r="D13" s="281"/>
+      <c r="E13" s="281"/>
+      <c r="F13" s="281"/>
+      <c r="G13" s="281"/>
+      <c r="H13" s="281"/>
+      <c r="I13" s="282"/>
     </row>
     <row r="14" spans="1:9" ht="66" customHeight="1">
       <c r="A14" s="165">
         <v>2</v>
       </c>
-      <c r="B14" s="318" t="s">
+      <c r="B14" s="283" t="s">
         <v>249</v>
       </c>
       <c r="C14" s="177" t="s">
@@ -7895,7 +7900,7 @@
         <f>A14+1</f>
         <v>3</v>
       </c>
-      <c r="B15" s="319"/>
+      <c r="B15" s="284"/>
       <c r="C15" s="166" t="s">
         <v>245</v>
       </c>
@@ -7917,7 +7922,7 @@
         <f>A15+1</f>
         <v>4</v>
       </c>
-      <c r="B16" s="319"/>
+      <c r="B16" s="284"/>
       <c r="C16" s="166" t="s">
         <v>247</v>
       </c>
@@ -7939,7 +7944,7 @@
         <f t="shared" ref="A17:A21" si="0">A16+1</f>
         <v>5</v>
       </c>
-      <c r="B17" s="319"/>
+      <c r="B17" s="284"/>
       <c r="C17" s="166" t="s">
         <v>248</v>
       </c>
@@ -7961,7 +7966,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B18" s="319"/>
+      <c r="B18" s="284"/>
       <c r="C18" s="166" t="s">
         <v>253</v>
       </c>
@@ -7983,7 +7988,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B19" s="319"/>
+      <c r="B19" s="284"/>
       <c r="C19" s="166" t="s">
         <v>255</v>
       </c>
@@ -8005,7 +8010,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B20" s="319"/>
+      <c r="B20" s="284"/>
       <c r="C20" s="166" t="s">
         <v>254</v>
       </c>
@@ -8027,7 +8032,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B21" s="320"/>
+      <c r="B21" s="285"/>
       <c r="C21" s="166" t="s">
         <v>256</v>
       </c>
@@ -8073,7 +8078,7 @@
         <f t="shared" ref="A23:A58" si="1">A22+1</f>
         <v>11</v>
       </c>
-      <c r="B23" s="321" t="s">
+      <c r="B23" s="286" t="s">
         <v>557</v>
       </c>
       <c r="C23" s="166" t="s">
@@ -8097,7 +8102,7 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B24" s="322"/>
+      <c r="B24" s="287"/>
       <c r="C24" s="166" t="s">
         <v>558</v>
       </c>
@@ -8119,7 +8124,7 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B25" s="322"/>
+      <c r="B25" s="287"/>
       <c r="C25" s="166" t="s">
         <v>579</v>
       </c>
@@ -8141,7 +8146,7 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B26" s="322"/>
+      <c r="B26" s="287"/>
       <c r="C26" s="166" t="s">
         <v>275</v>
       </c>
@@ -8163,7 +8168,7 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B27" s="322"/>
+      <c r="B27" s="287"/>
       <c r="C27" s="166" t="s">
         <v>493</v>
       </c>
@@ -8185,7 +8190,7 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B28" s="322"/>
+      <c r="B28" s="287"/>
       <c r="C28" s="166" t="s">
         <v>277</v>
       </c>
@@ -8207,7 +8212,7 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B29" s="322"/>
+      <c r="B29" s="287"/>
       <c r="C29" s="166" t="s">
         <v>278</v>
       </c>
@@ -8229,7 +8234,7 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B30" s="322"/>
+      <c r="B30" s="287"/>
       <c r="C30" s="166" t="s">
         <v>279</v>
       </c>
@@ -8457,7 +8462,7 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B40" s="321" t="s">
+      <c r="B40" s="286" t="s">
         <v>583</v>
       </c>
       <c r="C40" s="166" t="s">
@@ -8481,7 +8486,7 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B41" s="322"/>
+      <c r="B41" s="287"/>
       <c r="C41" s="166" t="s">
         <v>558</v>
       </c>
@@ -8503,7 +8508,7 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B42" s="322"/>
+      <c r="B42" s="287"/>
       <c r="C42" s="166" t="s">
         <v>579</v>
       </c>
@@ -8525,7 +8530,7 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B43" s="322"/>
+      <c r="B43" s="287"/>
       <c r="C43" s="166" t="s">
         <v>275</v>
       </c>
@@ -8547,7 +8552,7 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B44" s="322"/>
+      <c r="B44" s="287"/>
       <c r="C44" s="166" t="s">
         <v>493</v>
       </c>
@@ -8569,7 +8574,7 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B45" s="322"/>
+      <c r="B45" s="287"/>
       <c r="C45" s="166" t="s">
         <v>277</v>
       </c>
@@ -8591,7 +8596,7 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B46" s="322"/>
+      <c r="B46" s="287"/>
       <c r="C46" s="166" t="s">
         <v>278</v>
       </c>
@@ -8613,7 +8618,7 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B47" s="322"/>
+      <c r="B47" s="287"/>
       <c r="C47" s="166" t="s">
         <v>279</v>
       </c>
@@ -8880,6 +8885,19 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="B23:B30"/>
     <mergeCell ref="B56:B58"/>
     <mergeCell ref="B40:B47"/>
@@ -8889,19 +8907,6 @@
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="B14:B21"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12 F14:F58">
@@ -9453,13 +9458,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F1FB9E11-3D79-46CC-BED1-C4F060AFC065}" topLeftCell="A20">
-      <selection activeCell="A21" sqref="A21"/>
+    <customSheetView guid="{FD5FE319-AD9E-494D-BEEE-D43E425D7630}">
+      <selection activeCell="H21" sqref="H21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{FD5FE319-AD9E-494D-BEEE-D43E425D7630}">
-      <selection activeCell="H21" sqref="H21"/>
+    <customSheetView guid="{F1FB9E11-3D79-46CC-BED1-C4F060AFC065}" topLeftCell="A20">
+      <selection activeCell="A21" sqref="A21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
     </customSheetView>
@@ -9509,10 +9514,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:314" s="12" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A1" s="258" t="s">
+      <c r="A1" s="268" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="258"/>
+      <c r="B1" s="268"/>
       <c r="C1" s="41"/>
       <c r="D1" s="23"/>
       <c r="E1" s="42"/>
@@ -9521,76 +9526,76 @@
       <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:314" s="7" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A2" s="259" t="s">
+      <c r="A2" s="269" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="260"/>
-      <c r="C2" s="261" t="s">
+      <c r="B2" s="270"/>
+      <c r="C2" s="271" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="262"/>
-      <c r="E2" s="262"/>
-      <c r="F2" s="263"/>
-      <c r="G2" s="263"/>
-      <c r="H2" s="264"/>
+      <c r="D2" s="272"/>
+      <c r="E2" s="272"/>
+      <c r="F2" s="273"/>
+      <c r="G2" s="273"/>
+      <c r="H2" s="274"/>
     </row>
     <row r="3" spans="1:314" s="7" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A3" s="265" t="s">
+      <c r="A3" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="266"/>
-      <c r="C3" s="267" t="s">
+      <c r="B3" s="254"/>
+      <c r="C3" s="275" t="s">
         <v>152</v>
       </c>
-      <c r="D3" s="268"/>
-      <c r="E3" s="268"/>
-      <c r="F3" s="269"/>
-      <c r="G3" s="269"/>
-      <c r="H3" s="270"/>
+      <c r="D3" s="276"/>
+      <c r="E3" s="276"/>
+      <c r="F3" s="277"/>
+      <c r="G3" s="277"/>
+      <c r="H3" s="278"/>
     </row>
     <row r="4" spans="1:314" s="7" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A4" s="265" t="s">
+      <c r="A4" s="253" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="266"/>
-      <c r="C4" s="277" t="s">
+      <c r="B4" s="254"/>
+      <c r="C4" s="255" t="s">
         <v>229</v>
       </c>
-      <c r="D4" s="278"/>
+      <c r="D4" s="256"/>
       <c r="E4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="247"/>
-      <c r="G4" s="248"/>
-      <c r="H4" s="249"/>
+      <c r="F4" s="257"/>
+      <c r="G4" s="258"/>
+      <c r="H4" s="259"/>
     </row>
     <row r="5" spans="1:314" s="7" customFormat="1" ht="15">
-      <c r="A5" s="250" t="s">
+      <c r="A5" s="260" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="251"/>
-      <c r="C5" s="251"/>
-      <c r="D5" s="251"/>
-      <c r="E5" s="251"/>
-      <c r="F5" s="252"/>
-      <c r="G5" s="252"/>
-      <c r="H5" s="253"/>
+      <c r="B5" s="261"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="262"/>
+      <c r="G5" s="262"/>
+      <c r="H5" s="263"/>
     </row>
     <row r="6" spans="1:314" s="7" customFormat="1" ht="15">
-      <c r="A6" s="254" t="s">
+      <c r="A6" s="264" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="255"/>
+      <c r="B6" s="265"/>
       <c r="C6" s="25"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
-      <c r="F6" s="256"/>
-      <c r="G6" s="256"/>
-      <c r="H6" s="257"/>
+      <c r="F6" s="266"/>
+      <c r="G6" s="266"/>
+      <c r="H6" s="267"/>
     </row>
     <row r="7" spans="1:314" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="271"/>
-      <c r="B7" s="272"/>
+      <c r="A7" s="247"/>
+      <c r="B7" s="248"/>
       <c r="C7" s="28" t="s">
         <v>7</v>
       </c>
@@ -9611,10 +9616,10 @@
       </c>
     </row>
     <row r="8" spans="1:314" s="7" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A8" s="273" t="s">
+      <c r="A8" s="249" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="274"/>
+      <c r="B8" s="250"/>
       <c r="C8" s="27">
         <f>COUNTIF(F13:F53,"Passed")</f>
         <v>0</v>
@@ -9638,10 +9643,10 @@
       </c>
     </row>
     <row r="9" spans="1:314" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1">
-      <c r="A9" s="275" t="s">
+      <c r="A9" s="251" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="276"/>
+      <c r="B9" s="252"/>
       <c r="C9" s="27">
         <f xml:space="preserve"> COUNTIF(G13:G53,"Passed")</f>
         <v>0</v>
@@ -19876,11 +19881,6 @@
     <filterColumn colId="5" showButton="0"/>
   </autoFilter>
   <mergeCells count="16">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A6:B6"/>
@@ -19892,6 +19892,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E499:E1048576">
@@ -19942,10 +19947,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:314" s="12" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A1" s="258" t="s">
+      <c r="A1" s="268" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="258"/>
+      <c r="B1" s="268"/>
       <c r="C1" s="41"/>
       <c r="D1" s="23"/>
       <c r="E1" s="42"/>
@@ -19954,76 +19959,76 @@
       <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:314" s="7" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A2" s="259" t="s">
+      <c r="A2" s="269" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="260"/>
-      <c r="C2" s="261" t="s">
+      <c r="B2" s="270"/>
+      <c r="C2" s="271" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="262"/>
-      <c r="E2" s="262"/>
-      <c r="F2" s="263"/>
-      <c r="G2" s="263"/>
-      <c r="H2" s="264"/>
+      <c r="D2" s="272"/>
+      <c r="E2" s="272"/>
+      <c r="F2" s="273"/>
+      <c r="G2" s="273"/>
+      <c r="H2" s="274"/>
     </row>
     <row r="3" spans="1:314" s="7" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A3" s="265" t="s">
+      <c r="A3" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="266"/>
-      <c r="C3" s="267" t="s">
+      <c r="B3" s="254"/>
+      <c r="C3" s="275" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="268"/>
-      <c r="E3" s="268"/>
-      <c r="F3" s="269"/>
-      <c r="G3" s="269"/>
-      <c r="H3" s="270"/>
+      <c r="D3" s="276"/>
+      <c r="E3" s="276"/>
+      <c r="F3" s="277"/>
+      <c r="G3" s="277"/>
+      <c r="H3" s="278"/>
     </row>
     <row r="4" spans="1:314" s="7" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A4" s="265" t="s">
+      <c r="A4" s="253" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="266"/>
-      <c r="C4" s="277" t="s">
+      <c r="B4" s="254"/>
+      <c r="C4" s="255" t="s">
         <v>229</v>
       </c>
-      <c r="D4" s="278"/>
+      <c r="D4" s="256"/>
       <c r="E4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="247"/>
-      <c r="G4" s="248"/>
-      <c r="H4" s="249"/>
+      <c r="F4" s="257"/>
+      <c r="G4" s="258"/>
+      <c r="H4" s="259"/>
     </row>
     <row r="5" spans="1:314" s="7" customFormat="1" ht="15">
-      <c r="A5" s="250" t="s">
+      <c r="A5" s="260" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="251"/>
-      <c r="C5" s="251"/>
-      <c r="D5" s="251"/>
-      <c r="E5" s="251"/>
-      <c r="F5" s="252"/>
-      <c r="G5" s="252"/>
-      <c r="H5" s="253"/>
+      <c r="B5" s="261"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="262"/>
+      <c r="G5" s="262"/>
+      <c r="H5" s="263"/>
     </row>
     <row r="6" spans="1:314" s="7" customFormat="1" ht="15">
-      <c r="A6" s="254" t="s">
+      <c r="A6" s="264" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="255"/>
+      <c r="B6" s="265"/>
       <c r="C6" s="25"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
-      <c r="F6" s="256"/>
-      <c r="G6" s="256"/>
-      <c r="H6" s="257"/>
+      <c r="F6" s="266"/>
+      <c r="G6" s="266"/>
+      <c r="H6" s="267"/>
     </row>
     <row r="7" spans="1:314" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="271"/>
-      <c r="B7" s="272"/>
+      <c r="A7" s="247"/>
+      <c r="B7" s="248"/>
       <c r="C7" s="28" t="s">
         <v>7</v>
       </c>
@@ -20038,10 +20043,10 @@
       </c>
     </row>
     <row r="8" spans="1:314" s="7" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A8" s="273" t="s">
+      <c r="A8" s="249" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="274"/>
+      <c r="B8" s="250"/>
       <c r="C8" s="27">
         <f>COUNTIF(F12:F31,"Passed")</f>
         <v>17</v>
@@ -20060,10 +20065,10 @@
       </c>
     </row>
     <row r="9" spans="1:314" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1">
-      <c r="A9" s="275" t="s">
+      <c r="A9" s="251" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="276"/>
+      <c r="B9" s="252"/>
       <c r="C9" s="27">
         <f xml:space="preserve"> COUNTIF(G12:G31,"Passed")</f>
         <v>0</v>
@@ -27823,10 +27828,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:314" s="12" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A1" s="258" t="s">
+      <c r="A1" s="268" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="258"/>
+      <c r="B1" s="268"/>
       <c r="C1" s="41"/>
       <c r="D1" s="23"/>
       <c r="E1" s="42"/>
@@ -27835,76 +27840,76 @@
       <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:314" s="7" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A2" s="259" t="s">
+      <c r="A2" s="269" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="260"/>
-      <c r="C2" s="261" t="s">
+      <c r="B2" s="270"/>
+      <c r="C2" s="271" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="262"/>
-      <c r="E2" s="262"/>
-      <c r="F2" s="263"/>
-      <c r="G2" s="263"/>
-      <c r="H2" s="264"/>
+      <c r="D2" s="272"/>
+      <c r="E2" s="272"/>
+      <c r="F2" s="273"/>
+      <c r="G2" s="273"/>
+      <c r="H2" s="274"/>
     </row>
     <row r="3" spans="1:314" s="7" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A3" s="265" t="s">
+      <c r="A3" s="253" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="266"/>
-      <c r="C3" s="267" t="s">
+      <c r="B3" s="254"/>
+      <c r="C3" s="275" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="268"/>
-      <c r="E3" s="268"/>
-      <c r="F3" s="269"/>
-      <c r="G3" s="269"/>
-      <c r="H3" s="270"/>
+      <c r="D3" s="276"/>
+      <c r="E3" s="276"/>
+      <c r="F3" s="277"/>
+      <c r="G3" s="277"/>
+      <c r="H3" s="278"/>
     </row>
     <row r="4" spans="1:314" s="7" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A4" s="265" t="s">
+      <c r="A4" s="253" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="266"/>
-      <c r="C4" s="277" t="s">
+      <c r="B4" s="254"/>
+      <c r="C4" s="255" t="s">
         <v>229</v>
       </c>
-      <c r="D4" s="278"/>
+      <c r="D4" s="256"/>
       <c r="E4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="247"/>
-      <c r="G4" s="248"/>
-      <c r="H4" s="249"/>
+      <c r="F4" s="257"/>
+      <c r="G4" s="258"/>
+      <c r="H4" s="259"/>
     </row>
     <row r="5" spans="1:314" s="7" customFormat="1" ht="15">
-      <c r="A5" s="250" t="s">
+      <c r="A5" s="260" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="251"/>
-      <c r="C5" s="251"/>
-      <c r="D5" s="251"/>
-      <c r="E5" s="251"/>
-      <c r="F5" s="252"/>
-      <c r="G5" s="252"/>
-      <c r="H5" s="253"/>
+      <c r="B5" s="261"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="262"/>
+      <c r="G5" s="262"/>
+      <c r="H5" s="263"/>
     </row>
     <row r="6" spans="1:314" s="7" customFormat="1" ht="15">
-      <c r="A6" s="254" t="s">
+      <c r="A6" s="264" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="255"/>
+      <c r="B6" s="265"/>
       <c r="C6" s="25"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
-      <c r="F6" s="256"/>
-      <c r="G6" s="256"/>
-      <c r="H6" s="257"/>
+      <c r="F6" s="266"/>
+      <c r="G6" s="266"/>
+      <c r="H6" s="267"/>
     </row>
     <row r="7" spans="1:314" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="271"/>
-      <c r="B7" s="272"/>
+      <c r="A7" s="247"/>
+      <c r="B7" s="248"/>
       <c r="C7" s="28" t="s">
         <v>7</v>
       </c>
@@ -27919,10 +27924,10 @@
       </c>
     </row>
     <row r="8" spans="1:314" s="7" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A8" s="273" t="s">
+      <c r="A8" s="249" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="274"/>
+      <c r="B8" s="250"/>
       <c r="C8" s="27">
         <f>COUNTIF(F12:F15,"Passed")</f>
         <v>0</v>
@@ -27941,10 +27946,10 @@
       </c>
     </row>
     <row r="9" spans="1:314" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1">
-      <c r="A9" s="275" t="s">
+      <c r="A9" s="251" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="276"/>
+      <c r="B9" s="252"/>
       <c r="C9" s="27">
         <f xml:space="preserve"> COUNTIF(G12:G15,"Passed")</f>
         <v>0</v>
@@ -35945,11 +35950,6 @@
     <filterColumn colId="5" showButton="0"/>
   </autoFilter>
   <mergeCells count="16">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A6:B6"/>
@@ -35961,6 +35961,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E463:E1048576">
@@ -36005,10 +36010,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:315" s="142" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="321" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="279"/>
+      <c r="B1" s="321"/>
       <c r="C1" s="139"/>
       <c r="D1" s="139"/>
       <c r="E1" s="140"/>
@@ -36016,81 +36021,81 @@
       <c r="I1" s="143"/>
     </row>
     <row r="2" spans="1:315" s="142" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A2" s="280" t="s">
+      <c r="A2" s="322" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="281"/>
+      <c r="B2" s="323"/>
       <c r="C2" s="144"/>
-      <c r="D2" s="282" t="s">
+      <c r="D2" s="324" t="s">
         <v>230</v>
       </c>
-      <c r="E2" s="283"/>
-      <c r="F2" s="283"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="285"/>
+      <c r="E2" s="325"/>
+      <c r="F2" s="325"/>
+      <c r="G2" s="326"/>
+      <c r="H2" s="326"/>
+      <c r="I2" s="327"/>
     </row>
     <row r="3" spans="1:315" s="142" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A3" s="286" t="s">
+      <c r="A3" s="306" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="287"/>
+      <c r="B3" s="307"/>
       <c r="C3" s="145"/>
-      <c r="D3" s="288" t="s">
+      <c r="D3" s="328" t="s">
         <v>237</v>
       </c>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="290"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="291"/>
+      <c r="E3" s="329"/>
+      <c r="F3" s="329"/>
+      <c r="G3" s="330"/>
+      <c r="H3" s="330"/>
+      <c r="I3" s="331"/>
     </row>
     <row r="4" spans="1:315" s="142" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A4" s="286" t="s">
+      <c r="A4" s="306" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="287"/>
+      <c r="B4" s="307"/>
       <c r="C4" s="145"/>
-      <c r="D4" s="301" t="s">
+      <c r="D4" s="308" t="s">
         <v>229</v>
       </c>
-      <c r="E4" s="302"/>
+      <c r="E4" s="309"/>
       <c r="F4" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="303"/>
-      <c r="H4" s="304"/>
-      <c r="I4" s="305"/>
+      <c r="G4" s="310"/>
+      <c r="H4" s="311"/>
+      <c r="I4" s="312"/>
     </row>
     <row r="5" spans="1:315" s="142" customFormat="1" ht="12.75">
-      <c r="A5" s="306" t="s">
+      <c r="A5" s="313" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="307"/>
-      <c r="C5" s="307"/>
-      <c r="D5" s="307"/>
-      <c r="E5" s="307"/>
-      <c r="F5" s="307"/>
-      <c r="G5" s="308"/>
-      <c r="H5" s="308"/>
-      <c r="I5" s="309"/>
+      <c r="B5" s="314"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="314"/>
+      <c r="E5" s="314"/>
+      <c r="F5" s="314"/>
+      <c r="G5" s="315"/>
+      <c r="H5" s="315"/>
+      <c r="I5" s="316"/>
     </row>
     <row r="6" spans="1:315" s="142" customFormat="1" ht="12.75">
-      <c r="A6" s="310" t="s">
+      <c r="A6" s="317" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="311"/>
+      <c r="B6" s="318"/>
       <c r="C6" s="147"/>
       <c r="D6" s="148"/>
       <c r="E6" s="149"/>
       <c r="F6" s="149"/>
-      <c r="G6" s="312"/>
-      <c r="H6" s="312"/>
-      <c r="I6" s="313"/>
+      <c r="G6" s="319"/>
+      <c r="H6" s="319"/>
+      <c r="I6" s="320"/>
     </row>
     <row r="7" spans="1:315" s="142" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="292"/>
-      <c r="B7" s="293"/>
+      <c r="A7" s="297"/>
+      <c r="B7" s="298"/>
       <c r="C7" s="147"/>
       <c r="D7" s="150" t="s">
         <v>7</v>
@@ -36106,10 +36111,10 @@
       </c>
     </row>
     <row r="8" spans="1:315" s="142" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A8" s="294" t="s">
+      <c r="A8" s="299" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="295"/>
+      <c r="B8" s="300"/>
       <c r="C8" s="154"/>
       <c r="D8" s="148">
         <f>COUNTIF(G12:G14,"Passed")</f>
@@ -36129,10 +36134,10 @@
       </c>
     </row>
     <row r="9" spans="1:315" s="142" customFormat="1" ht="21" customHeight="1" thickBot="1">
-      <c r="A9" s="296" t="s">
+      <c r="A9" s="301" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="297"/>
+      <c r="B9" s="302"/>
       <c r="C9" s="155"/>
       <c r="D9" s="156">
         <f xml:space="preserve"> COUNTIF(H12:H14,"Passed")</f>
@@ -36487,17 +36492,17 @@
       <c r="LC10" s="158"/>
     </row>
     <row r="11" spans="1:315" s="173" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="298" t="s">
+      <c r="A11" s="303" t="s">
         <v>240</v>
       </c>
-      <c r="B11" s="299"/>
-      <c r="C11" s="299"/>
-      <c r="D11" s="299"/>
-      <c r="E11" s="299"/>
-      <c r="F11" s="299"/>
-      <c r="G11" s="299"/>
-      <c r="H11" s="299"/>
-      <c r="I11" s="300"/>
+      <c r="B11" s="304"/>
+      <c r="C11" s="304"/>
+      <c r="D11" s="304"/>
+      <c r="E11" s="304"/>
+      <c r="F11" s="304"/>
+      <c r="G11" s="304"/>
+      <c r="H11" s="304"/>
+      <c r="I11" s="305"/>
       <c r="J11" s="159"/>
       <c r="K11" s="159"/>
       <c r="L11" s="159"/>
@@ -36853,17 +36858,17 @@
       <c r="AI12" s="163"/>
     </row>
     <row r="13" spans="1:315" s="173" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="315" t="s">
+      <c r="A13" s="280" t="s">
         <v>235</v>
       </c>
-      <c r="B13" s="316"/>
-      <c r="C13" s="316"/>
-      <c r="D13" s="316"/>
-      <c r="E13" s="316"/>
-      <c r="F13" s="316"/>
-      <c r="G13" s="316"/>
-      <c r="H13" s="316"/>
-      <c r="I13" s="317"/>
+      <c r="B13" s="281"/>
+      <c r="C13" s="281"/>
+      <c r="D13" s="281"/>
+      <c r="E13" s="281"/>
+      <c r="F13" s="281"/>
+      <c r="G13" s="281"/>
+      <c r="H13" s="281"/>
+      <c r="I13" s="282"/>
       <c r="J13" s="159"/>
       <c r="K13" s="159"/>
       <c r="L13" s="159"/>
@@ -37175,7 +37180,7 @@
       <c r="A14" s="165">
         <v>2</v>
       </c>
-      <c r="B14" s="318" t="s">
+      <c r="B14" s="283" t="s">
         <v>249</v>
       </c>
       <c r="C14" s="177" t="s">
@@ -37230,7 +37235,7 @@
         <f>A14+1</f>
         <v>3</v>
       </c>
-      <c r="B15" s="319"/>
+      <c r="B15" s="284"/>
       <c r="C15" s="166" t="s">
         <v>245</v>
       </c>
@@ -37283,7 +37288,7 @@
         <f>A15+1</f>
         <v>4</v>
       </c>
-      <c r="B16" s="319"/>
+      <c r="B16" s="284"/>
       <c r="C16" s="166" t="s">
         <v>247</v>
       </c>
@@ -37336,7 +37341,7 @@
         <f t="shared" ref="A17:A37" si="0">A16+1</f>
         <v>5</v>
       </c>
-      <c r="B17" s="319"/>
+      <c r="B17" s="284"/>
       <c r="C17" s="166" t="s">
         <v>248</v>
       </c>
@@ -37364,7 +37369,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B18" s="319"/>
+      <c r="B18" s="284"/>
       <c r="C18" s="166" t="s">
         <v>253</v>
       </c>
@@ -37392,7 +37397,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B19" s="319"/>
+      <c r="B19" s="284"/>
       <c r="C19" s="166" t="s">
         <v>255</v>
       </c>
@@ -37420,7 +37425,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B20" s="319"/>
+      <c r="B20" s="284"/>
       <c r="C20" s="166" t="s">
         <v>254</v>
       </c>
@@ -37448,7 +37453,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B21" s="320"/>
+      <c r="B21" s="285"/>
       <c r="C21" s="166" t="s">
         <v>256</v>
       </c>
@@ -37506,7 +37511,7 @@
         <f>A22+1</f>
         <v>11</v>
       </c>
-      <c r="B23" s="321" t="s">
+      <c r="B23" s="286" t="s">
         <v>298</v>
       </c>
       <c r="C23" s="166" t="s">
@@ -37536,7 +37541,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B24" s="322"/>
+      <c r="B24" s="287"/>
       <c r="C24" s="169" t="s">
         <v>271</v>
       </c>
@@ -37562,7 +37567,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B25" s="322"/>
+      <c r="B25" s="287"/>
       <c r="C25" s="166" t="s">
         <v>283</v>
       </c>
@@ -37590,7 +37595,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B26" s="322"/>
+      <c r="B26" s="287"/>
       <c r="C26" s="166" t="s">
         <v>236</v>
       </c>
@@ -37618,7 +37623,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B27" s="322"/>
+      <c r="B27" s="287"/>
       <c r="C27" s="166" t="s">
         <v>275</v>
       </c>
@@ -37646,7 +37651,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B28" s="322"/>
+      <c r="B28" s="287"/>
       <c r="C28" s="166" t="s">
         <v>273</v>
       </c>
@@ -37674,7 +37679,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B29" s="322"/>
+      <c r="B29" s="287"/>
       <c r="C29" s="166" t="s">
         <v>277</v>
       </c>
@@ -37702,7 +37707,7 @@
         <f>A29+1</f>
         <v>18</v>
       </c>
-      <c r="B30" s="322"/>
+      <c r="B30" s="287"/>
       <c r="C30" s="166" t="s">
         <v>278</v>
       </c>
@@ -37730,7 +37735,7 @@
         <f>A30+1</f>
         <v>19</v>
       </c>
-      <c r="B31" s="322"/>
+      <c r="B31" s="287"/>
       <c r="C31" s="166" t="s">
         <v>279</v>
       </c>
@@ -37758,7 +37763,7 @@
         <f>A31+1</f>
         <v>20</v>
       </c>
-      <c r="B32" s="323" t="s">
+      <c r="B32" s="288" t="s">
         <v>354</v>
       </c>
       <c r="C32" s="166" t="s">
@@ -37788,7 +37793,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B33" s="324"/>
+      <c r="B33" s="289"/>
       <c r="C33" s="169" t="s">
         <v>271</v>
       </c>
@@ -37814,7 +37819,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B34" s="324"/>
+      <c r="B34" s="289"/>
       <c r="C34" s="166" t="s">
         <v>291</v>
       </c>
@@ -37842,7 +37847,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B35" s="324"/>
+      <c r="B35" s="289"/>
       <c r="C35" s="166" t="s">
         <v>236</v>
       </c>
@@ -37870,7 +37875,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B36" s="324"/>
+      <c r="B36" s="289"/>
       <c r="C36" s="166" t="s">
         <v>275</v>
       </c>
@@ -37898,7 +37903,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B37" s="324"/>
+      <c r="B37" s="289"/>
       <c r="C37" s="187" t="s">
         <v>273</v>
       </c>
@@ -37926,7 +37931,7 @@
         <f>A37+1</f>
         <v>26</v>
       </c>
-      <c r="B38" s="324"/>
+      <c r="B38" s="289"/>
       <c r="C38" s="177" t="s">
         <v>278</v>
       </c>
@@ -37954,7 +37959,7 @@
         <f>A38+1</f>
         <v>27</v>
       </c>
-      <c r="B39" s="325"/>
+      <c r="B39" s="290"/>
       <c r="C39" s="177" t="s">
         <v>277</v>
       </c>
@@ -38012,7 +38017,7 @@
         <f>A40+1</f>
         <v>29</v>
       </c>
-      <c r="B41" s="326" t="s">
+      <c r="B41" s="291" t="s">
         <v>310</v>
       </c>
       <c r="C41" s="198" t="s">
@@ -38042,7 +38047,7 @@
         <f t="shared" ref="A42:A58" si="1">A41+1</f>
         <v>30</v>
       </c>
-      <c r="B42" s="327"/>
+      <c r="B42" s="292"/>
       <c r="C42" s="132" t="s">
         <v>300</v>
       </c>
@@ -38070,7 +38075,7 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B43" s="327"/>
+      <c r="B43" s="292"/>
       <c r="C43" s="132" t="s">
         <v>301</v>
       </c>
@@ -38098,7 +38103,7 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B44" s="327"/>
+      <c r="B44" s="292"/>
       <c r="C44" s="132" t="s">
         <v>302</v>
       </c>
@@ -38126,7 +38131,7 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B45" s="327"/>
+      <c r="B45" s="292"/>
       <c r="C45" s="132" t="s">
         <v>307</v>
       </c>
@@ -38154,7 +38159,7 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B46" s="327"/>
+      <c r="B46" s="292"/>
       <c r="C46" s="132" t="s">
         <v>307</v>
       </c>
@@ -38182,7 +38187,7 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B47" s="327"/>
+      <c r="B47" s="292"/>
       <c r="C47" s="132" t="s">
         <v>302</v>
       </c>
@@ -38210,7 +38215,7 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B48" s="327"/>
+      <c r="B48" s="292"/>
       <c r="C48" s="132" t="s">
         <v>302</v>
       </c>
@@ -38238,7 +38243,7 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B49" s="328"/>
+      <c r="B49" s="293"/>
       <c r="C49" s="132" t="s">
         <v>307</v>
       </c>
@@ -38266,7 +38271,7 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B50" s="329" t="s">
+      <c r="B50" s="294" t="s">
         <v>318</v>
       </c>
       <c r="C50" s="166" t="s">
@@ -38296,7 +38301,7 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B51" s="330"/>
+      <c r="B51" s="295"/>
       <c r="C51" s="187" t="s">
         <v>273</v>
       </c>
@@ -38324,7 +38329,7 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B52" s="330"/>
+      <c r="B52" s="295"/>
       <c r="C52" s="177" t="s">
         <v>278</v>
       </c>
@@ -38352,7 +38357,7 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B53" s="330"/>
+      <c r="B53" s="295"/>
       <c r="C53" s="177" t="s">
         <v>277</v>
       </c>
@@ -38380,7 +38385,7 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B54" s="330"/>
+      <c r="B54" s="295"/>
       <c r="C54" s="166" t="s">
         <v>236</v>
       </c>
@@ -38408,7 +38413,7 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B55" s="331"/>
+      <c r="B55" s="296"/>
       <c r="C55" s="166" t="s">
         <v>275</v>
       </c>
@@ -38436,7 +38441,7 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B56" s="314" t="s">
+      <c r="B56" s="279" t="s">
         <v>320</v>
       </c>
       <c r="C56" s="166" t="s">
@@ -38466,7 +38471,7 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B57" s="314"/>
+      <c r="B57" s="279"/>
       <c r="C57" s="166" t="s">
         <v>327</v>
       </c>
@@ -38494,7 +38499,7 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B58" s="314"/>
+      <c r="B58" s="279"/>
       <c r="C58" s="166" t="s">
         <v>328</v>
       </c>
@@ -38519,13 +38524,13 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="B23:B31"/>
-    <mergeCell ref="B32:B39"/>
-    <mergeCell ref="B41:B49"/>
-    <mergeCell ref="B50:B55"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
@@ -38536,13 +38541,13 @@
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="B23:B31"/>
+    <mergeCell ref="B32:B39"/>
+    <mergeCell ref="B41:B49"/>
+    <mergeCell ref="B50:B55"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12 F14:F58">
@@ -38580,10 +38585,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="321" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="279"/>
+      <c r="B1" s="321"/>
       <c r="C1" s="184"/>
       <c r="D1" s="184"/>
       <c r="E1" s="140"/>
@@ -38593,81 +38598,81 @@
       <c r="I1" s="143"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="280" t="s">
+      <c r="A2" s="322" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="281"/>
+      <c r="B2" s="323"/>
       <c r="C2" s="144"/>
-      <c r="D2" s="282" t="s">
+      <c r="D2" s="324" t="s">
         <v>230</v>
       </c>
-      <c r="E2" s="283"/>
-      <c r="F2" s="283"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="285"/>
+      <c r="E2" s="325"/>
+      <c r="F2" s="325"/>
+      <c r="G2" s="326"/>
+      <c r="H2" s="326"/>
+      <c r="I2" s="327"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="286" t="s">
+      <c r="A3" s="306" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="287"/>
+      <c r="B3" s="307"/>
       <c r="C3" s="145"/>
-      <c r="D3" s="288" t="s">
+      <c r="D3" s="328" t="s">
         <v>329</v>
       </c>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="290"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="291"/>
+      <c r="E3" s="329"/>
+      <c r="F3" s="329"/>
+      <c r="G3" s="330"/>
+      <c r="H3" s="330"/>
+      <c r="I3" s="331"/>
     </row>
     <row r="4" spans="1:9" ht="25.5">
-      <c r="A4" s="286" t="s">
+      <c r="A4" s="306" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="287"/>
+      <c r="B4" s="307"/>
       <c r="C4" s="145"/>
-      <c r="D4" s="301" t="s">
+      <c r="D4" s="308" t="s">
         <v>229</v>
       </c>
-      <c r="E4" s="302"/>
+      <c r="E4" s="309"/>
       <c r="F4" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="303"/>
-      <c r="H4" s="304"/>
-      <c r="I4" s="305"/>
+      <c r="G4" s="310"/>
+      <c r="H4" s="311"/>
+      <c r="I4" s="312"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="306" t="s">
+      <c r="A5" s="313" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="307"/>
-      <c r="C5" s="307"/>
-      <c r="D5" s="307"/>
-      <c r="E5" s="307"/>
-      <c r="F5" s="307"/>
-      <c r="G5" s="308"/>
-      <c r="H5" s="308"/>
-      <c r="I5" s="309"/>
+      <c r="B5" s="314"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="314"/>
+      <c r="E5" s="314"/>
+      <c r="F5" s="314"/>
+      <c r="G5" s="315"/>
+      <c r="H5" s="315"/>
+      <c r="I5" s="316"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="310" t="s">
+      <c r="A6" s="317" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="311"/>
+      <c r="B6" s="318"/>
       <c r="C6" s="147"/>
       <c r="D6" s="148"/>
       <c r="E6" s="149"/>
       <c r="F6" s="149"/>
-      <c r="G6" s="312"/>
-      <c r="H6" s="312"/>
-      <c r="I6" s="313"/>
+      <c r="G6" s="319"/>
+      <c r="H6" s="319"/>
+      <c r="I6" s="320"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="292"/>
-      <c r="B7" s="293"/>
+      <c r="A7" s="297"/>
+      <c r="B7" s="298"/>
       <c r="C7" s="147"/>
       <c r="D7" s="150" t="s">
         <v>7</v>
@@ -38685,10 +38690,10 @@
       <c r="I7" s="142"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="294" t="s">
+      <c r="A8" s="299" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="295"/>
+      <c r="B8" s="300"/>
       <c r="C8" s="154"/>
       <c r="D8" s="148">
         <f>COUNTIF(G12:G14,"Passed")</f>
@@ -38710,10 +38715,10 @@
       <c r="I8" s="142"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="296" t="s">
+      <c r="A9" s="301" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="297"/>
+      <c r="B9" s="302"/>
       <c r="C9" s="155"/>
       <c r="D9" s="156">
         <f xml:space="preserve"> COUNTIF(H12:H14,"Passed")</f>
@@ -38764,17 +38769,17 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="298" t="s">
+      <c r="A11" s="303" t="s">
         <v>240</v>
       </c>
-      <c r="B11" s="299"/>
-      <c r="C11" s="299"/>
-      <c r="D11" s="299"/>
-      <c r="E11" s="299"/>
-      <c r="F11" s="299"/>
-      <c r="G11" s="299"/>
-      <c r="H11" s="299"/>
-      <c r="I11" s="300"/>
+      <c r="B11" s="304"/>
+      <c r="C11" s="304"/>
+      <c r="D11" s="304"/>
+      <c r="E11" s="304"/>
+      <c r="F11" s="304"/>
+      <c r="G11" s="304"/>
+      <c r="H11" s="304"/>
+      <c r="I11" s="305"/>
     </row>
     <row r="12" spans="1:9" ht="75" customHeight="1">
       <c r="A12" s="161">
@@ -38798,23 +38803,23 @@
       <c r="I12" s="162"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="315" t="s">
+      <c r="A13" s="280" t="s">
         <v>333</v>
       </c>
-      <c r="B13" s="316"/>
-      <c r="C13" s="316"/>
-      <c r="D13" s="316"/>
-      <c r="E13" s="316"/>
-      <c r="F13" s="316"/>
-      <c r="G13" s="316"/>
-      <c r="H13" s="316"/>
-      <c r="I13" s="317"/>
+      <c r="B13" s="281"/>
+      <c r="C13" s="281"/>
+      <c r="D13" s="281"/>
+      <c r="E13" s="281"/>
+      <c r="F13" s="281"/>
+      <c r="G13" s="281"/>
+      <c r="H13" s="281"/>
+      <c r="I13" s="282"/>
     </row>
     <row r="14" spans="1:9" ht="90" customHeight="1">
       <c r="A14" s="165">
         <v>2</v>
       </c>
-      <c r="B14" s="318" t="s">
+      <c r="B14" s="283" t="s">
         <v>249</v>
       </c>
       <c r="C14" s="177" t="s">
@@ -38838,7 +38843,7 @@
         <f>A14+1</f>
         <v>3</v>
       </c>
-      <c r="B15" s="319"/>
+      <c r="B15" s="284"/>
       <c r="C15" s="166" t="s">
         <v>245</v>
       </c>
@@ -38860,7 +38865,7 @@
         <f>A15+1</f>
         <v>4</v>
       </c>
-      <c r="B16" s="319"/>
+      <c r="B16" s="284"/>
       <c r="C16" s="166" t="s">
         <v>247</v>
       </c>
@@ -38882,7 +38887,7 @@
         <f t="shared" ref="A17:A37" si="0">A16+1</f>
         <v>5</v>
       </c>
-      <c r="B17" s="319"/>
+      <c r="B17" s="284"/>
       <c r="C17" s="166" t="s">
         <v>248</v>
       </c>
@@ -38904,7 +38909,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B18" s="319"/>
+      <c r="B18" s="284"/>
       <c r="C18" s="166" t="s">
         <v>253</v>
       </c>
@@ -38926,7 +38931,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B19" s="319"/>
+      <c r="B19" s="284"/>
       <c r="C19" s="166" t="s">
         <v>255</v>
       </c>
@@ -38948,7 +38953,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B20" s="319"/>
+      <c r="B20" s="284"/>
       <c r="C20" s="166" t="s">
         <v>254</v>
       </c>
@@ -38970,7 +38975,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B21" s="320"/>
+      <c r="B21" s="285"/>
       <c r="C21" s="166" t="s">
         <v>256</v>
       </c>
@@ -39016,7 +39021,7 @@
         <f>A22+1</f>
         <v>11</v>
       </c>
-      <c r="B23" s="321" t="s">
+      <c r="B23" s="286" t="s">
         <v>365</v>
       </c>
       <c r="C23" s="166" t="s">
@@ -39040,7 +39045,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B24" s="322"/>
+      <c r="B24" s="287"/>
       <c r="C24" s="169" t="s">
         <v>271</v>
       </c>
@@ -39060,7 +39065,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B25" s="322"/>
+      <c r="B25" s="287"/>
       <c r="C25" s="166" t="s">
         <v>369</v>
       </c>
@@ -39082,7 +39087,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B26" s="322"/>
+      <c r="B26" s="287"/>
       <c r="C26" s="166" t="s">
         <v>236</v>
       </c>
@@ -39104,7 +39109,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B27" s="322"/>
+      <c r="B27" s="287"/>
       <c r="C27" s="166" t="s">
         <v>275</v>
       </c>
@@ -39126,7 +39131,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B28" s="322"/>
+      <c r="B28" s="287"/>
       <c r="C28" s="166" t="s">
         <v>273</v>
       </c>
@@ -39148,7 +39153,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B29" s="322"/>
+      <c r="B29" s="287"/>
       <c r="C29" s="166" t="s">
         <v>277</v>
       </c>
@@ -39170,7 +39175,7 @@
         <f>A29+1</f>
         <v>18</v>
       </c>
-      <c r="B30" s="322"/>
+      <c r="B30" s="287"/>
       <c r="C30" s="166" t="s">
         <v>278</v>
       </c>
@@ -39192,7 +39197,7 @@
         <f>A30+1</f>
         <v>19</v>
       </c>
-      <c r="B31" s="322"/>
+      <c r="B31" s="287"/>
       <c r="C31" s="166" t="s">
         <v>279</v>
       </c>
@@ -39214,7 +39219,7 @@
         <f>A31+1</f>
         <v>20</v>
       </c>
-      <c r="B32" s="323" t="s">
+      <c r="B32" s="288" t="s">
         <v>374</v>
       </c>
       <c r="C32" s="166" t="s">
@@ -39238,7 +39243,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B33" s="324"/>
+      <c r="B33" s="289"/>
       <c r="C33" s="169" t="s">
         <v>271</v>
       </c>
@@ -39258,7 +39263,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B34" s="324"/>
+      <c r="B34" s="289"/>
       <c r="C34" s="166" t="s">
         <v>369</v>
       </c>
@@ -39280,7 +39285,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B35" s="324"/>
+      <c r="B35" s="289"/>
       <c r="C35" s="166" t="s">
         <v>236</v>
       </c>
@@ -39302,7 +39307,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B36" s="324"/>
+      <c r="B36" s="289"/>
       <c r="C36" s="166" t="s">
         <v>275</v>
       </c>
@@ -39324,7 +39329,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B37" s="324"/>
+      <c r="B37" s="289"/>
       <c r="C37" s="187" t="s">
         <v>273</v>
       </c>
@@ -39346,7 +39351,7 @@
         <f>A37+1</f>
         <v>26</v>
       </c>
-      <c r="B38" s="324"/>
+      <c r="B38" s="289"/>
       <c r="C38" s="177" t="s">
         <v>278</v>
       </c>
@@ -39368,7 +39373,7 @@
         <f>A38+1</f>
         <v>27</v>
       </c>
-      <c r="B39" s="325"/>
+      <c r="B39" s="290"/>
       <c r="C39" s="177" t="s">
         <v>277</v>
       </c>
@@ -39414,7 +39419,7 @@
         <f>A40+1</f>
         <v>29</v>
       </c>
-      <c r="B41" s="326" t="s">
+      <c r="B41" s="291" t="s">
         <v>379</v>
       </c>
       <c r="C41" s="198" t="s">
@@ -39438,7 +39443,7 @@
         <f t="shared" ref="A42:A57" si="1">A41+1</f>
         <v>30</v>
       </c>
-      <c r="B42" s="327"/>
+      <c r="B42" s="292"/>
       <c r="C42" s="132" t="s">
         <v>383</v>
       </c>
@@ -39460,7 +39465,7 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B43" s="327"/>
+      <c r="B43" s="292"/>
       <c r="C43" s="132" t="s">
         <v>384</v>
       </c>
@@ -39482,7 +39487,7 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B44" s="327"/>
+      <c r="B44" s="292"/>
       <c r="C44" s="132" t="s">
         <v>385</v>
       </c>
@@ -39504,7 +39509,7 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B45" s="327"/>
+      <c r="B45" s="292"/>
       <c r="C45" s="132" t="s">
         <v>389</v>
       </c>
@@ -39526,7 +39531,7 @@
         <f>A45+1</f>
         <v>34</v>
       </c>
-      <c r="B46" s="327"/>
+      <c r="B46" s="292"/>
       <c r="C46" s="132" t="s">
         <v>315</v>
       </c>
@@ -39548,7 +39553,7 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B47" s="327"/>
+      <c r="B47" s="292"/>
       <c r="C47" s="132" t="s">
         <v>388</v>
       </c>
@@ -39570,7 +39575,7 @@
         <f>A47+1</f>
         <v>36</v>
       </c>
-      <c r="B48" s="329" t="s">
+      <c r="B48" s="294" t="s">
         <v>391</v>
       </c>
       <c r="C48" s="166" t="s">
@@ -39594,7 +39599,7 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B49" s="330"/>
+      <c r="B49" s="295"/>
       <c r="C49" s="187" t="s">
         <v>273</v>
       </c>
@@ -39616,7 +39621,7 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B50" s="330"/>
+      <c r="B50" s="295"/>
       <c r="C50" s="177" t="s">
         <v>278</v>
       </c>
@@ -39638,7 +39643,7 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B51" s="330"/>
+      <c r="B51" s="295"/>
       <c r="C51" s="177" t="s">
         <v>277</v>
       </c>
@@ -39660,7 +39665,7 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B52" s="330"/>
+      <c r="B52" s="295"/>
       <c r="C52" s="166" t="s">
         <v>236</v>
       </c>
@@ -39679,7 +39684,7 @@
     </row>
     <row r="53" spans="1:9" ht="90" customHeight="1">
       <c r="A53" s="197"/>
-      <c r="B53" s="330"/>
+      <c r="B53" s="295"/>
       <c r="C53" s="166" t="s">
         <v>399</v>
       </c>
@@ -39701,7 +39706,7 @@
         <f>A52+1</f>
         <v>41</v>
       </c>
-      <c r="B54" s="331"/>
+      <c r="B54" s="296"/>
       <c r="C54" s="166" t="s">
         <v>275</v>
       </c>
@@ -39723,7 +39728,7 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B55" s="314" t="s">
+      <c r="B55" s="279" t="s">
         <v>320</v>
       </c>
       <c r="C55" s="166" t="s">
@@ -39747,7 +39752,7 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B56" s="314"/>
+      <c r="B56" s="279"/>
       <c r="C56" s="166" t="s">
         <v>327</v>
       </c>
@@ -39769,7 +39774,7 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B57" s="314"/>
+      <c r="B57" s="279"/>
       <c r="C57" s="166" t="s">
         <v>328</v>
       </c>
@@ -39788,13 +39793,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B23:B31"/>
+    <mergeCell ref="B32:B39"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="B48:B54"/>
+    <mergeCell ref="B55:B57"/>
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D4:E4"/>
@@ -39807,11 +39810,13 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A13:I13"/>
-    <mergeCell ref="B23:B31"/>
-    <mergeCell ref="B32:B39"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G3 G5:G6 G10">
@@ -39850,10 +39855,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="321" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="279"/>
+      <c r="B1" s="321"/>
       <c r="C1" s="194"/>
       <c r="D1" s="194"/>
       <c r="E1" s="140"/>
@@ -39863,81 +39868,81 @@
       <c r="I1" s="143"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="280" t="s">
+      <c r="A2" s="322" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="281"/>
+      <c r="B2" s="323"/>
       <c r="C2" s="144"/>
-      <c r="D2" s="282" t="s">
+      <c r="D2" s="324" t="s">
         <v>230</v>
       </c>
-      <c r="E2" s="283"/>
-      <c r="F2" s="283"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="285"/>
+      <c r="E2" s="325"/>
+      <c r="F2" s="325"/>
+      <c r="G2" s="326"/>
+      <c r="H2" s="326"/>
+      <c r="I2" s="327"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="286" t="s">
+      <c r="A3" s="306" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="287"/>
+      <c r="B3" s="307"/>
       <c r="C3" s="145"/>
-      <c r="D3" s="288" t="s">
+      <c r="D3" s="328" t="s">
         <v>402</v>
       </c>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="290"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="291"/>
+      <c r="E3" s="329"/>
+      <c r="F3" s="329"/>
+      <c r="G3" s="330"/>
+      <c r="H3" s="330"/>
+      <c r="I3" s="331"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="286" t="s">
+      <c r="A4" s="306" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="287"/>
+      <c r="B4" s="307"/>
       <c r="C4" s="145"/>
-      <c r="D4" s="301" t="s">
+      <c r="D4" s="308" t="s">
         <v>229</v>
       </c>
-      <c r="E4" s="302"/>
+      <c r="E4" s="309"/>
       <c r="F4" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="303"/>
-      <c r="H4" s="304"/>
-      <c r="I4" s="305"/>
+      <c r="G4" s="310"/>
+      <c r="H4" s="311"/>
+      <c r="I4" s="312"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="306" t="s">
+      <c r="A5" s="313" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="307"/>
-      <c r="C5" s="307"/>
-      <c r="D5" s="307"/>
-      <c r="E5" s="307"/>
-      <c r="F5" s="307"/>
-      <c r="G5" s="308"/>
-      <c r="H5" s="308"/>
-      <c r="I5" s="309"/>
+      <c r="B5" s="314"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="314"/>
+      <c r="E5" s="314"/>
+      <c r="F5" s="314"/>
+      <c r="G5" s="315"/>
+      <c r="H5" s="315"/>
+      <c r="I5" s="316"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="310" t="s">
+      <c r="A6" s="317" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="311"/>
+      <c r="B6" s="318"/>
       <c r="C6" s="147"/>
       <c r="D6" s="148"/>
       <c r="E6" s="149"/>
       <c r="F6" s="149"/>
-      <c r="G6" s="312"/>
-      <c r="H6" s="312"/>
-      <c r="I6" s="313"/>
+      <c r="G6" s="319"/>
+      <c r="H6" s="319"/>
+      <c r="I6" s="320"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="292"/>
-      <c r="B7" s="293"/>
+      <c r="A7" s="297"/>
+      <c r="B7" s="298"/>
       <c r="C7" s="147"/>
       <c r="D7" s="150" t="s">
         <v>7</v>
@@ -39955,10 +39960,10 @@
       <c r="I7" s="142"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="294" t="s">
+      <c r="A8" s="299" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="295"/>
+      <c r="B8" s="300"/>
       <c r="C8" s="154"/>
       <c r="D8" s="148">
         <f>COUNTIF(G12:G14,"Passed")</f>
@@ -39980,10 +39985,10 @@
       <c r="I8" s="142"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="296" t="s">
+      <c r="A9" s="301" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="297"/>
+      <c r="B9" s="302"/>
       <c r="C9" s="155"/>
       <c r="D9" s="156">
         <f xml:space="preserve"> COUNTIF(H12:H14,"Passed")</f>
@@ -40034,17 +40039,17 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="298" t="s">
+      <c r="A11" s="303" t="s">
         <v>460</v>
       </c>
-      <c r="B11" s="299"/>
-      <c r="C11" s="299"/>
-      <c r="D11" s="299"/>
-      <c r="E11" s="299"/>
-      <c r="F11" s="299"/>
-      <c r="G11" s="299"/>
-      <c r="H11" s="299"/>
-      <c r="I11" s="300"/>
+      <c r="B11" s="304"/>
+      <c r="C11" s="304"/>
+      <c r="D11" s="304"/>
+      <c r="E11" s="304"/>
+      <c r="F11" s="304"/>
+      <c r="G11" s="304"/>
+      <c r="H11" s="304"/>
+      <c r="I11" s="305"/>
     </row>
     <row r="12" spans="1:9" ht="63" customHeight="1">
       <c r="A12" s="161">
@@ -40068,23 +40073,23 @@
       <c r="I12" s="162"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="315" t="s">
+      <c r="A13" s="280" t="s">
         <v>333</v>
       </c>
-      <c r="B13" s="316"/>
-      <c r="C13" s="316"/>
-      <c r="D13" s="316"/>
-      <c r="E13" s="316"/>
-      <c r="F13" s="316"/>
-      <c r="G13" s="316"/>
-      <c r="H13" s="316"/>
-      <c r="I13" s="317"/>
+      <c r="B13" s="281"/>
+      <c r="C13" s="281"/>
+      <c r="D13" s="281"/>
+      <c r="E13" s="281"/>
+      <c r="F13" s="281"/>
+      <c r="G13" s="281"/>
+      <c r="H13" s="281"/>
+      <c r="I13" s="282"/>
     </row>
     <row r="14" spans="1:9" ht="66" customHeight="1">
       <c r="A14" s="165">
         <v>2</v>
       </c>
-      <c r="B14" s="318" t="s">
+      <c r="B14" s="283" t="s">
         <v>249</v>
       </c>
       <c r="C14" s="177" t="s">
@@ -40108,7 +40113,7 @@
         <f>A14+1</f>
         <v>3</v>
       </c>
-      <c r="B15" s="319"/>
+      <c r="B15" s="284"/>
       <c r="C15" s="166" t="s">
         <v>245</v>
       </c>
@@ -40130,7 +40135,7 @@
         <f>A15+1</f>
         <v>4</v>
       </c>
-      <c r="B16" s="319"/>
+      <c r="B16" s="284"/>
       <c r="C16" s="166" t="s">
         <v>247</v>
       </c>
@@ -40152,7 +40157,7 @@
         <f t="shared" ref="A17:A37" si="0">A16+1</f>
         <v>5</v>
       </c>
-      <c r="B17" s="319"/>
+      <c r="B17" s="284"/>
       <c r="C17" s="166" t="s">
         <v>248</v>
       </c>
@@ -40174,7 +40179,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B18" s="319"/>
+      <c r="B18" s="284"/>
       <c r="C18" s="166" t="s">
         <v>253</v>
       </c>
@@ -40196,7 +40201,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B19" s="319"/>
+      <c r="B19" s="284"/>
       <c r="C19" s="166" t="s">
         <v>255</v>
       </c>
@@ -40218,7 +40223,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B20" s="319"/>
+      <c r="B20" s="284"/>
       <c r="C20" s="166" t="s">
         <v>254</v>
       </c>
@@ -40240,7 +40245,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B21" s="320"/>
+      <c r="B21" s="285"/>
       <c r="C21" s="166" t="s">
         <v>256</v>
       </c>
@@ -40286,7 +40291,7 @@
         <f>A22+1</f>
         <v>11</v>
       </c>
-      <c r="B23" s="321" t="s">
+      <c r="B23" s="286" t="s">
         <v>442</v>
       </c>
       <c r="C23" s="166" t="s">
@@ -40310,7 +40315,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B24" s="322"/>
+      <c r="B24" s="287"/>
       <c r="C24" s="169" t="s">
         <v>271</v>
       </c>
@@ -40330,7 +40335,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B25" s="322"/>
+      <c r="B25" s="287"/>
       <c r="C25" s="166" t="s">
         <v>369</v>
       </c>
@@ -40352,7 +40357,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B26" s="322"/>
+      <c r="B26" s="287"/>
       <c r="C26" s="166" t="s">
         <v>236</v>
       </c>
@@ -40374,7 +40379,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B27" s="322"/>
+      <c r="B27" s="287"/>
       <c r="C27" s="166" t="s">
         <v>275</v>
       </c>
@@ -40396,7 +40401,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B28" s="322"/>
+      <c r="B28" s="287"/>
       <c r="C28" s="166" t="s">
         <v>273</v>
       </c>
@@ -40418,7 +40423,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B29" s="322"/>
+      <c r="B29" s="287"/>
       <c r="C29" s="166" t="s">
         <v>277</v>
       </c>
@@ -40440,7 +40445,7 @@
         <f>A29+1</f>
         <v>18</v>
       </c>
-      <c r="B30" s="322"/>
+      <c r="B30" s="287"/>
       <c r="C30" s="166" t="s">
         <v>278</v>
       </c>
@@ -40462,7 +40467,7 @@
         <f>A30+1</f>
         <v>19</v>
       </c>
-      <c r="B31" s="322"/>
+      <c r="B31" s="287"/>
       <c r="C31" s="166" t="s">
         <v>279</v>
       </c>
@@ -40484,7 +40489,7 @@
         <f>A31+1</f>
         <v>20</v>
       </c>
-      <c r="B32" s="323" t="s">
+      <c r="B32" s="288" t="s">
         <v>439</v>
       </c>
       <c r="C32" s="166" t="s">
@@ -40508,7 +40513,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B33" s="324"/>
+      <c r="B33" s="289"/>
       <c r="C33" s="169" t="s">
         <v>271</v>
       </c>
@@ -40528,7 +40533,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B34" s="324"/>
+      <c r="B34" s="289"/>
       <c r="C34" s="166" t="s">
         <v>369</v>
       </c>
@@ -40550,7 +40555,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B35" s="324"/>
+      <c r="B35" s="289"/>
       <c r="C35" s="166" t="s">
         <v>236</v>
       </c>
@@ -40572,7 +40577,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B36" s="324"/>
+      <c r="B36" s="289"/>
       <c r="C36" s="166" t="s">
         <v>275</v>
       </c>
@@ -40594,7 +40599,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B37" s="324"/>
+      <c r="B37" s="289"/>
       <c r="C37" s="187" t="s">
         <v>273</v>
       </c>
@@ -40616,7 +40621,7 @@
         <f>A37+1</f>
         <v>26</v>
       </c>
-      <c r="B38" s="324"/>
+      <c r="B38" s="289"/>
       <c r="C38" s="177" t="s">
         <v>278</v>
       </c>
@@ -40638,7 +40643,7 @@
         <f>A38+1</f>
         <v>27</v>
       </c>
-      <c r="B39" s="325"/>
+      <c r="B39" s="290"/>
       <c r="C39" s="177" t="s">
         <v>277</v>
       </c>
@@ -40684,7 +40689,7 @@
         <f>A40+1</f>
         <v>29</v>
       </c>
-      <c r="B41" s="326" t="s">
+      <c r="B41" s="291" t="s">
         <v>443</v>
       </c>
       <c r="C41" s="198" t="s">
@@ -40708,7 +40713,7 @@
         <f t="shared" ref="A42:A59" si="1">A41+1</f>
         <v>30</v>
       </c>
-      <c r="B42" s="327"/>
+      <c r="B42" s="292"/>
       <c r="C42" s="132" t="s">
         <v>445</v>
       </c>
@@ -40730,7 +40735,7 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B43" s="327"/>
+      <c r="B43" s="292"/>
       <c r="C43" s="132" t="s">
         <v>446</v>
       </c>
@@ -40752,7 +40757,7 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B44" s="327"/>
+      <c r="B44" s="292"/>
       <c r="C44" s="132" t="s">
         <v>448</v>
       </c>
@@ -40774,7 +40779,7 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B45" s="327"/>
+      <c r="B45" s="292"/>
       <c r="C45" s="132" t="s">
         <v>449</v>
       </c>
@@ -40796,7 +40801,7 @@
         <f>A45+1</f>
         <v>34</v>
       </c>
-      <c r="B46" s="327"/>
+      <c r="B46" s="292"/>
       <c r="C46" s="132" t="s">
         <v>315</v>
       </c>
@@ -40818,7 +40823,7 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B47" s="327"/>
+      <c r="B47" s="292"/>
       <c r="C47" s="132" t="s">
         <v>450</v>
       </c>
@@ -40840,7 +40845,7 @@
         <f>A47+1</f>
         <v>36</v>
       </c>
-      <c r="B48" s="329" t="s">
+      <c r="B48" s="294" t="s">
         <v>456</v>
       </c>
       <c r="C48" s="166" t="s">
@@ -40864,7 +40869,7 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B49" s="330"/>
+      <c r="B49" s="295"/>
       <c r="C49" s="187" t="s">
         <v>273</v>
       </c>
@@ -40886,7 +40891,7 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B50" s="330"/>
+      <c r="B50" s="295"/>
       <c r="C50" s="177" t="s">
         <v>278</v>
       </c>
@@ -40908,7 +40913,7 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B51" s="330"/>
+      <c r="B51" s="295"/>
       <c r="C51" s="177" t="s">
         <v>277</v>
       </c>
@@ -40930,7 +40935,7 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B52" s="330"/>
+      <c r="B52" s="295"/>
       <c r="C52" s="166" t="s">
         <v>236</v>
       </c>
@@ -40952,7 +40957,7 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B53" s="330"/>
+      <c r="B53" s="295"/>
       <c r="C53" s="166" t="s">
         <v>399</v>
       </c>
@@ -40974,7 +40979,7 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B54" s="330"/>
+      <c r="B54" s="295"/>
       <c r="C54" s="187" t="s">
         <v>275</v>
       </c>
@@ -41018,7 +41023,7 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B56" s="331"/>
+      <c r="B56" s="296"/>
       <c r="C56" s="132" t="s">
         <v>105</v>
       </c>
@@ -41045,7 +41050,7 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B57" s="314"/>
+      <c r="B57" s="279"/>
       <c r="C57" s="216" t="s">
         <v>327</v>
       </c>
@@ -41067,7 +41072,7 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B58" s="314"/>
+      <c r="B58" s="279"/>
       <c r="C58" s="166" t="s">
         <v>326</v>
       </c>
@@ -41089,7 +41094,7 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B59" s="314"/>
+      <c r="B59" s="279"/>
       <c r="C59" s="166" t="s">
         <v>328</v>
       </c>
@@ -41108,11 +41113,13 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B23:B31"/>
-    <mergeCell ref="B32:B39"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="B48:B56"/>
-    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
     <mergeCell ref="B14:B21"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D4:E4"/>
@@ -41125,13 +41132,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="B23:B31"/>
+    <mergeCell ref="B32:B39"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="B48:B56"/>
+    <mergeCell ref="B57:B59"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12 F14:F59">
@@ -41167,10 +41172,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="321" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="279"/>
+      <c r="B1" s="321"/>
       <c r="C1" s="208"/>
       <c r="D1" s="208"/>
       <c r="E1" s="140"/>
@@ -41180,81 +41185,81 @@
       <c r="I1" s="143"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="280" t="s">
+      <c r="A2" s="322" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="281"/>
+      <c r="B2" s="323"/>
       <c r="C2" s="144"/>
-      <c r="D2" s="282" t="s">
+      <c r="D2" s="324" t="s">
         <v>230</v>
       </c>
-      <c r="E2" s="283"/>
-      <c r="F2" s="283"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="284"/>
-      <c r="I2" s="285"/>
+      <c r="E2" s="325"/>
+      <c r="F2" s="325"/>
+      <c r="G2" s="326"/>
+      <c r="H2" s="326"/>
+      <c r="I2" s="327"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="286" t="s">
+      <c r="A3" s="306" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="287"/>
+      <c r="B3" s="307"/>
       <c r="C3" s="145"/>
-      <c r="D3" s="288" t="s">
+      <c r="D3" s="328" t="s">
         <v>461</v>
       </c>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="290"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="291"/>
+      <c r="E3" s="329"/>
+      <c r="F3" s="329"/>
+      <c r="G3" s="330"/>
+      <c r="H3" s="330"/>
+      <c r="I3" s="331"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="286" t="s">
+      <c r="A4" s="306" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="287"/>
+      <c r="B4" s="307"/>
       <c r="C4" s="145"/>
-      <c r="D4" s="301" t="s">
+      <c r="D4" s="308" t="s">
         <v>229</v>
       </c>
-      <c r="E4" s="302"/>
+      <c r="E4" s="309"/>
       <c r="F4" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="303"/>
-      <c r="H4" s="304"/>
-      <c r="I4" s="305"/>
+      <c r="G4" s="310"/>
+      <c r="H4" s="311"/>
+      <c r="I4" s="312"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="306" t="s">
+      <c r="A5" s="313" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="307"/>
-      <c r="C5" s="307"/>
-      <c r="D5" s="307"/>
-      <c r="E5" s="307"/>
-      <c r="F5" s="307"/>
-      <c r="G5" s="308"/>
-      <c r="H5" s="308"/>
-      <c r="I5" s="309"/>
+      <c r="B5" s="314"/>
+      <c r="C5" s="314"/>
+      <c r="D5" s="314"/>
+      <c r="E5" s="314"/>
+      <c r="F5" s="314"/>
+      <c r="G5" s="315"/>
+      <c r="H5" s="315"/>
+      <c r="I5" s="316"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="310" t="s">
+      <c r="A6" s="317" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="311"/>
+      <c r="B6" s="318"/>
       <c r="C6" s="147"/>
       <c r="D6" s="148"/>
       <c r="E6" s="149"/>
       <c r="F6" s="149"/>
-      <c r="G6" s="312"/>
-      <c r="H6" s="312"/>
-      <c r="I6" s="313"/>
+      <c r="G6" s="319"/>
+      <c r="H6" s="319"/>
+      <c r="I6" s="320"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="292"/>
-      <c r="B7" s="293"/>
+      <c r="A7" s="297"/>
+      <c r="B7" s="298"/>
       <c r="C7" s="147"/>
       <c r="D7" s="150" t="s">
         <v>7</v>
@@ -41272,10 +41277,10 @@
       <c r="I7" s="142"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="294" t="s">
+      <c r="A8" s="299" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="295"/>
+      <c r="B8" s="300"/>
       <c r="C8" s="154"/>
       <c r="D8" s="148">
         <f>COUNTIF(G12:G14,"Passed")</f>
@@ -41297,10 +41302,10 @@
       <c r="I8" s="142"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="296" t="s">
+      <c r="A9" s="301" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="297"/>
+      <c r="B9" s="302"/>
       <c r="C9" s="155"/>
       <c r="D9" s="156">
         <f xml:space="preserve"> COUNTIF(H12:H14,"Passed")</f>
@@ -41351,17 +41356,17 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="298" t="s">
+      <c r="A11" s="303" t="s">
         <v>462</v>
       </c>
-      <c r="B11" s="299"/>
-      <c r="C11" s="299"/>
-      <c r="D11" s="299"/>
-      <c r="E11" s="299"/>
-      <c r="F11" s="299"/>
-      <c r="G11" s="299"/>
-      <c r="H11" s="299"/>
-      <c r="I11" s="300"/>
+      <c r="B11" s="304"/>
+      <c r="C11" s="304"/>
+      <c r="D11" s="304"/>
+      <c r="E11" s="304"/>
+      <c r="F11" s="304"/>
+      <c r="G11" s="304"/>
+      <c r="H11" s="304"/>
+      <c r="I11" s="305"/>
     </row>
     <row r="12" spans="1:9" ht="63" customHeight="1">
       <c r="A12" s="161">
@@ -41385,23 +41390,23 @@
       <c r="I12" s="162"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="315" t="s">
+      <c r="A13" s="280" t="s">
         <v>333</v>
       </c>
-      <c r="B13" s="316"/>
-      <c r="C13" s="316"/>
-      <c r="D13" s="316"/>
-      <c r="E13" s="316"/>
-      <c r="F13" s="316"/>
-      <c r="G13" s="316"/>
-      <c r="H13" s="316"/>
-      <c r="I13" s="317"/>
+      <c r="B13" s="281"/>
+      <c r="C13" s="281"/>
+      <c r="D13" s="281"/>
+      <c r="E13" s="281"/>
+      <c r="F13" s="281"/>
+      <c r="G13" s="281"/>
+      <c r="H13" s="281"/>
+      <c r="I13" s="282"/>
     </row>
     <row r="14" spans="1:9" ht="66" customHeight="1">
       <c r="A14" s="165">
         <v>2</v>
       </c>
-      <c r="B14" s="318" t="s">
+      <c r="B14" s="283" t="s">
         <v>249</v>
       </c>
       <c r="C14" s="177" t="s">
@@ -41425,7 +41430,7 @@
         <f>A14+1</f>
         <v>3</v>
       </c>
-      <c r="B15" s="319"/>
+      <c r="B15" s="284"/>
       <c r="C15" s="166" t="s">
         <v>245</v>
       </c>
@@ -41447,7 +41452,7 @@
         <f>A15+1</f>
         <v>4</v>
       </c>
-      <c r="B16" s="319"/>
+      <c r="B16" s="284"/>
       <c r="C16" s="166" t="s">
         <v>247</v>
       </c>
@@ -41469,7 +41474,7 @@
         <f t="shared" ref="A17:A21" si="0">A16+1</f>
         <v>5</v>
       </c>
-      <c r="B17" s="319"/>
+      <c r="B17" s="284"/>
       <c r="C17" s="166" t="s">
         <v>248</v>
       </c>
@@ -41491,7 +41496,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B18" s="319"/>
+      <c r="B18" s="284"/>
       <c r="C18" s="166" t="s">
         <v>253</v>
       </c>
@@ -41513,7 +41518,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B19" s="319"/>
+      <c r="B19" s="284"/>
       <c r="C19" s="166" t="s">
         <v>255</v>
       </c>
@@ -41535,7 +41540,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B20" s="319"/>
+      <c r="B20" s="284"/>
       <c r="C20" s="166" t="s">
         <v>254</v>
       </c>
@@ -41557,7 +41562,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B21" s="320"/>
+      <c r="B21" s="285"/>
       <c r="C21" s="166" t="s">
         <v>256</v>
       </c>
@@ -41603,7 +41608,7 @@
         <f t="shared" ref="A23:A58" si="1">A22+1</f>
         <v>11</v>
       </c>
-      <c r="B23" s="321" t="s">
+      <c r="B23" s="286" t="s">
         <v>495</v>
       </c>
       <c r="C23" s="166" t="s">
@@ -41627,7 +41632,7 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B24" s="322"/>
+      <c r="B24" s="287"/>
       <c r="C24" s="166" t="s">
         <v>492</v>
       </c>
@@ -41649,7 +41654,7 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B25" s="322"/>
+      <c r="B25" s="287"/>
       <c r="C25" s="166" t="s">
         <v>236</v>
       </c>
@@ -41671,7 +41676,7 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B26" s="322"/>
+      <c r="B26" s="287"/>
       <c r="C26" s="166" t="s">
         <v>275</v>
       </c>
@@ -41693,7 +41698,7 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B27" s="322"/>
+      <c r="B27" s="287"/>
       <c r="C27" s="166" t="s">
         <v>493</v>
       </c>
@@ -41715,7 +41720,7 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B28" s="322"/>
+      <c r="B28" s="287"/>
       <c r="C28" s="166" t="s">
         <v>277</v>
       </c>
@@ -41737,7 +41742,7 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B29" s="322"/>
+      <c r="B29" s="287"/>
       <c r="C29" s="166" t="s">
         <v>278</v>
       </c>
@@ -41759,7 +41764,7 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B30" s="322"/>
+      <c r="B30" s="287"/>
       <c r="C30" s="166" t="s">
         <v>279</v>
       </c>
@@ -42209,7 +42214,7 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B50" s="330"/>
+      <c r="B50" s="295"/>
       <c r="C50" s="132" t="s">
         <v>184</v>
       </c>
@@ -42231,7 +42236,7 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B51" s="330"/>
+      <c r="B51" s="295"/>
       <c r="C51" s="132" t="s">
         <v>58</v>
       </c>
@@ -42253,7 +42258,7 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B52" s="330"/>
+      <c r="B52" s="295"/>
       <c r="C52" s="132" t="s">
         <v>132</v>
       </c>
@@ -42275,7 +42280,7 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B53" s="330"/>
+      <c r="B53" s="295"/>
       <c r="C53" s="132" t="s">
         <v>41</v>
       </c>
@@ -42319,7 +42324,7 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B55" s="331"/>
+      <c r="B55" s="296"/>
       <c r="C55" s="132" t="s">
         <v>105</v>
       </c>
@@ -42346,7 +42351,7 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B56" s="314"/>
+      <c r="B56" s="279"/>
       <c r="C56" s="216" t="s">
         <v>327</v>
       </c>
@@ -42368,7 +42373,7 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B57" s="314"/>
+      <c r="B57" s="279"/>
       <c r="C57" s="166" t="s">
         <v>326</v>
       </c>
@@ -42390,7 +42395,7 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B58" s="314"/>
+      <c r="B58" s="279"/>
       <c r="C58" s="166" t="s">
         <v>328</v>
       </c>
@@ -42409,6 +42414,19 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="B23:B30"/>
     <mergeCell ref="B40:B46"/>
     <mergeCell ref="B47:B55"/>
@@ -42419,19 +42437,6 @@
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="B14:B21"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G3 G5:G6 G10">

</xml_diff>